<commit_message>
updated syncs, updated datasheet
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyRequestor_RecnUnrecieve_MultipleLines.xlsx
+++ b/src/test/resources/datasheets/VerifyRequestor_RecnUnrecieve_MultipleLines.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="6210"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RecnUnrecieve_MultipleLines" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -25,187 +24,187 @@
     <t>Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Item Description </t>
+  </si>
+  <si>
+    <t>UNSPSC Code</t>
+  </si>
+  <si>
+    <t>Suggested Supplier(s)</t>
+  </si>
+  <si>
+    <t>Category Type</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Manufacturer Name</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit of Measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price </t>
+  </si>
+  <si>
+    <t>ChangeType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SelectCC </t>
+  </si>
+  <si>
+    <t>Role1</t>
+  </si>
+  <si>
+    <t>TaxType</t>
+  </si>
+  <si>
+    <t>TaxCode</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>ExpectedMsg</t>
+  </si>
+  <si>
+    <t>ExpectedStatus</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>Role2</t>
+  </si>
+  <si>
+    <t>Uprice</t>
+  </si>
+  <si>
+    <t>Uquantity</t>
+  </si>
+  <si>
+    <t>LeadTime</t>
+  </si>
+  <si>
+    <t>FreightID</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>CurrentView</t>
+  </si>
+  <si>
+    <t>ActiveIndex</t>
+  </si>
+  <si>
+    <t>ReceivingAgentRole</t>
+  </si>
+  <si>
+    <t>PkgSlipNumber</t>
+  </si>
+  <si>
+    <t>REQUESTOR</t>
+  </si>
+  <si>
+    <t>XEEVA -MJ</t>
+  </si>
+  <si>
+    <t>REPOFLOR 100 MG</t>
+  </si>
+  <si>
+    <t>UNSPSC001</t>
+  </si>
+  <si>
+    <t>Sachin Supplier Magna</t>
+  </si>
+  <si>
+    <t>INFORMATION TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>HARDWARE</t>
+  </si>
+  <si>
+    <t>CELL PHONES</t>
+  </si>
+  <si>
+    <t>ARMSTRONG</t>
+  </si>
+  <si>
+    <t>MPN001</t>
+  </si>
+  <si>
+    <t>1;2</t>
+  </si>
+  <si>
+    <t>EA-EACH;CU-CUBIC</t>
+  </si>
+  <si>
+    <t>1;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">headerlevel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMCOMERCIAL </t>
+  </si>
+  <si>
+    <t>BUYER</t>
+  </si>
+  <si>
+    <t>Test-Test</t>
+  </si>
+  <si>
+    <t>Test_usage-test</t>
+  </si>
+  <si>
+    <t>Desktops</t>
+  </si>
+  <si>
+    <t>ON-HOLD;Waiting for Approval</t>
+  </si>
+  <si>
+    <t>Hold;UnHold</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>SUPPLIER</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>CIP</t>
+  </si>
+  <si>
+    <t>added comments</t>
+  </si>
+  <si>
+    <t>Myview</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>REQUESTOR_RECEIVING_AGENT</t>
   </si>
   <si>
-    <t>XEEVA -MJ</t>
-  </si>
-  <si>
-    <t>PkgSlipNumber</t>
-  </si>
-  <si>
     <t>PS123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item Description </t>
-  </si>
-  <si>
-    <t>UNSPSC Code</t>
-  </si>
-  <si>
-    <t>Suggested Supplier(s)</t>
-  </si>
-  <si>
-    <t>Category Type</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Sub Category</t>
-  </si>
-  <si>
-    <t>Manufacturer Name</t>
-  </si>
-  <si>
-    <t>Manufacturer Part Number</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Unit of Measure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price </t>
-  </si>
-  <si>
-    <t>ChangeType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SelectCC </t>
-  </si>
-  <si>
-    <t>Role1</t>
-  </si>
-  <si>
-    <t>TaxType</t>
-  </si>
-  <si>
-    <t>TaxCode</t>
-  </si>
-  <si>
-    <t>ItemName</t>
-  </si>
-  <si>
-    <t>ExpectedMsg</t>
-  </si>
-  <si>
-    <t>ExpectedStatus</t>
-  </si>
-  <si>
-    <t>supplier</t>
-  </si>
-  <si>
-    <t>Role2</t>
-  </si>
-  <si>
-    <t>Uprice</t>
-  </si>
-  <si>
-    <t>Uquantity</t>
-  </si>
-  <si>
-    <t>LeadTime</t>
-  </si>
-  <si>
-    <t>FreightID</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>CurrentView</t>
-  </si>
-  <si>
-    <t>ActiveIndex</t>
-  </si>
-  <si>
-    <t>REQUESTOR</t>
-  </si>
-  <si>
-    <t>REPOFLOR 100 MG</t>
-  </si>
-  <si>
-    <t>UNSPSC001</t>
-  </si>
-  <si>
-    <t>Sachin Supplier Magna</t>
-  </si>
-  <si>
-    <t>INFORMATION TECHNOLOGY</t>
-  </si>
-  <si>
-    <t>HARDWARE</t>
-  </si>
-  <si>
-    <t>CELL PHONES</t>
-  </si>
-  <si>
-    <t>ARMSTRONG</t>
-  </si>
-  <si>
-    <t>MPN001</t>
-  </si>
-  <si>
-    <t>1;2</t>
-  </si>
-  <si>
-    <t>EA-EACH;CU-CUBIC</t>
-  </si>
-  <si>
-    <t>1;10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">headerlevel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMCOMERCIAL </t>
-  </si>
-  <si>
-    <t>BUYER</t>
-  </si>
-  <si>
-    <t>Test-Test</t>
-  </si>
-  <si>
-    <t>Test_usage-test</t>
-  </si>
-  <si>
-    <t>Desktops</t>
-  </si>
-  <si>
-    <t>ON-HOLD;Waiting for Approval</t>
-  </si>
-  <si>
-    <t>Hold;UnHold</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>SUPPLIER</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>CIP</t>
-  </si>
-  <si>
-    <t>added comments</t>
-  </si>
-  <si>
-    <t>Myview</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>ReceivingAgentRole</t>
   </si>
 </sst>
 </file>
@@ -538,19 +537,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="31" max="31" width="30" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" t="s">
@@ -560,196 +553,194 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>42</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>43</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>44</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>45</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>46</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>47</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>49</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>50</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>51</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA2" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>58</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>59</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" t="s">
         <v>61</v>
       </c>
-      <c r="AE2" t="s">
-        <v>2</v>
-      </c>
       <c r="AF2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:32"/>
-    <row r="7" spans="1:32"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the test data for the test case - Verify_CreateInvoiceBySuppplier.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyRequestor_RecnUnrecieve_MultipleLines.xlsx
+++ b/src/test/resources/datasheets/VerifyRequestor_RecnUnrecieve_MultipleLines.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="6210"/>
+    <workbookView xWindow="0" yWindow="2850" windowWidth="12675" windowHeight="4710"/>
   </bookViews>
   <sheets>
     <sheet name="RecnUnrecieve_MultipleLines" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <oleSize ref="A1"/>
 </workbook>
 </file>
@@ -538,18 +538,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="31" max="31" width="30" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -748,8 +751,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:32"/>
-    <row r="7" spans="1:32"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>